<commit_message>
Bugfix in regional definition: RSAF and SAF were swapped in capital definition
</commit_message>
<xml_diff>
--- a/input/data/IMAGE regions.xlsx
+++ b/input/data/IMAGE regions.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pbleefomgeving-my.sharepoint.com/personal/wijstvdk_pbl_nl/Documents/Documenten/COACCH/Project-MIMOSA/input/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{A77AAC8F-3387-4411-B32C-9D53F2955B4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4541AEAB-DBCA-498C-B387-9B30F6001567}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{A77AAC8F-3387-4411-B32C-9D53F2955B4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5B020FEE-0553-4AB4-BC09-E25E0A563E39}"/>
   <bookViews>
-    <workbookView xWindow="-22212" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="-120" windowWidth="27930" windowHeight="18240" tabRatio="916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Country to region" sheetId="13" r:id="rId1"/>
     <sheet name="IMAGE Regions" sheetId="14" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Country to region'!$A$1:$D$240</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="481">
   <si>
     <t>Canada</t>
   </si>
@@ -2163,10 +2166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D240"/>
+  <dimension ref="A1:I259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="G244" sqref="G244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,10 +2199,10 @@
         <v>36</v>
       </c>
       <c r="C2" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2224,10 +2227,10 @@
         <v>58</v>
       </c>
       <c r="C4" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2504,10 +2507,10 @@
         <v>148</v>
       </c>
       <c r="C24" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2546,10 +2549,10 @@
         <v>156</v>
       </c>
       <c r="C27" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2602,10 +2605,10 @@
         <v>174</v>
       </c>
       <c r="C31" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2616,10 +2619,10 @@
         <v>69</v>
       </c>
       <c r="C32" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,10 +2731,10 @@
         <v>224</v>
       </c>
       <c r="C40">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2756,10 +2759,10 @@
         <v>231</v>
       </c>
       <c r="C42" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2770,10 +2773,10 @@
         <v>237</v>
       </c>
       <c r="C43" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2812,10 +2815,10 @@
         <v>263</v>
       </c>
       <c r="C46" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2826,10 +2829,10 @@
         <v>264</v>
       </c>
       <c r="C47" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4332,10 +4335,10 @@
         <v>165</v>
       </c>
       <c r="C155" s="4">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D155" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5520,7 +5523,24 @@
         <v>11</v>
       </c>
     </row>
+    <row r="258" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H258">
+        <v>10</v>
+      </c>
+      <c r="I258" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H259">
+        <v>26</v>
+      </c>
+      <c r="I259" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:D240" xr:uid="{377DE0D3-E3A4-4832-907A-B8CB3029D3BD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <customProperties>

</xml_diff>